<commit_message>
- Add columns 'Protein' and 'Ontogeny' to Individuals.xlsx - Extract code for ontogeny parsing to separate function - Ontogeny specification for individuals
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C34232-2DB7-41B3-A223-790B0A3DD89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19CEBB4-C8C3-4171-A5A1-FD2C40F33AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Human</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Container Path</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Ontogeny</t>
   </si>
 </sst>
 </file>
@@ -422,31 +428,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.46875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.17578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.46875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.46875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -468,8 +474,14 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -507,13 +519,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.52734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.703125" style="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -527,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -556,17 +568,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="151fa1d8706c0355297f81811bd06e6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85a3e53823607994162d1630ec2e7479" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -803,6 +804,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
   <ds:schemaRefs>
@@ -812,17 +824,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713C675-E25A-461C-9068-CC8E8BA72888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -839,4 +840,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Casting to character NA Fix test Individuals.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19CEBB4-C8C3-4171-A5A1-FD2C40F33AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412BC6C-0ABD-45B9-8C88-5691BD90ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,28 +431,28 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.52734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.46875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -519,13 +519,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,6 +568,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="151fa1d8706c0355297f81811bd06e6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85a3e53823607994162d1630ec2e7479" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -804,17 +815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
   <ds:schemaRefs>
@@ -824,6 +824,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713C675-E25A-461C-9068-CC8E8BA72888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -840,15 +851,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Add columns 'Protein' and 'Ontogeny' to Individuals.xlsx (#467)
* - Add columns 'Protein' and 'Ontogeny' to Individuals.xlsx
- Extract code for ontogeny parsing to separate function
- Ontogeny specification for individuals

* Casting to character NA
Fix test Individuals.xlsx

* plotIDs within parenthesis will not be split by ','

* Remove develop branch from appveyor.yml

* add develop back

* Fix splitting of plot ids

* Return correct names of missing data sets
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C34232-2DB7-41B3-A223-790B0A3DD89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412BC6C-0ABD-45B9-8C88-5691BD90ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Human</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Container Path</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Ontogeny</t>
   </si>
 </sst>
 </file>
@@ -422,31 +428,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.8203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.87890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.87890625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.46875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.17578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.52734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.46875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.46875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.46875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -468,8 +474,14 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -509,7 +521,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.52734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.703125" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add new entries in excel files to test populationTimeProfile ploting + Update tests
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412BC6C-0ABD-45B9-8C88-5691BD90ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C56A0-9AD0-4D06-8DDC-663DC7FEBC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="9015" windowWidth="12975" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualBiometrics" sheetId="1" r:id="rId1"/>
@@ -431,28 +431,28 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.87890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.41015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.52734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.46875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -519,13 +519,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.703125" style="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -559,26 +559,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="151fa1d8706c0355297f81811bd06e6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85a3e53823607994162d1630ec2e7479" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -815,26 +795,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713C675-E25A-461C-9068-CC8E8BA72888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -851,4 +832,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add nSD handling if defined in Plot.xlsx (#544)
* add nSD handling if defined in Plot.xlsx

* add nSD column

* Add new entries in excel files to test populationTimeProfile ploting
+ Update tests

* Limit the plotGrid to create so there is no error during rendering

* Suppress expected warning from test

* Add fig.showtext = TRUE (#546)
+ minor tweaks of font sizes and margins
+ setting of vignette chunk options for figures

* Rename nSD to nsd (to match ospsuite's argument)
+ Update NEWS

* Update ospsuite version required to 12.0.0
+ pkgdown::build_site()
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412BC6C-0ABD-45B9-8C88-5691BD90ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C56A0-9AD0-4D06-8DDC-663DC7FEBC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="9015" windowWidth="12975" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualBiometrics" sheetId="1" r:id="rId1"/>
@@ -431,28 +431,28 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.87890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.41015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.52734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.46875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -519,13 +519,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.703125" style="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -559,26 +559,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="151fa1d8706c0355297f81811bd06e6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85a3e53823607994162d1630ec2e7479" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -815,26 +795,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713C675-E25A-461C-9068-CC8E8BA72888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -851,4 +832,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pksim installation instruction (#543)
* Add instructions for PK-Sim installation (#538)

* fix VignetteIndexEntry

* Add fig.showtext = TRUE on all vignettes so the images are rendered properly using showtext
+ reduce axis titles font size just a bit

* pkgdown::build_site()

* Clean NEWS
 + Fix headers
 + Reorganize headers to keep only:
   - Breaking changes
   - Major changes
   - Minor improvements and bug fixes

* Add introduction

* Add global/project installation instructions
+
wrap text

* pkgdown::build_article("install-pksim")

* Update vignettes/install-pksim.Rmd

* pkgdown::build_article("install-pksim")

---------

Co-authored-by: PavelBal <pavel.balazki@gmail.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C56A0-9AD0-4D06-8DDC-663DC7FEBC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412BC6C-0ABD-45B9-8C88-5691BD90ED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="9015" windowWidth="12975" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualBiometrics" sheetId="1" r:id="rId1"/>
@@ -431,28 +431,28 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.29296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.52734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.46875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -519,13 +519,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -559,6 +559,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="151fa1d8706c0355297f81811bd06e6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85a3e53823607994162d1630ec2e7479" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -795,27 +815,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713C675-E25A-461C-9068-CC8E8BA72888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -832,23 +851,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>